<commit_message>
Add total costs for all modules
</commit_message>
<xml_diff>
--- a/project_list.xlsx
+++ b/project_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pbhaskar/Desktop/Projects/landbosse_public/LandBOSSE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5589BAC1-D086-2D4E-B4C0-EC208F3BC502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1BF43A-C401-7447-886D-7F2862E30076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="14360" xr2:uid="{CA848B2B-50AD-1141-9E6B-5049DCE507C8}"/>
   </bookViews>
@@ -179,10 +179,10 @@
     <t>Crane breakdown fraction</t>
   </si>
   <si>
-    <t>ge15_dist_165</t>
-  </si>
-  <si>
     <t>ge15_public</t>
+  </si>
+  <si>
+    <t>foundation_validation_ge15</t>
   </si>
 </sst>
 </file>
@@ -238,23 +238,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -566,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978C2AE7-DAF9-A64F-82B2-BFC05FEB6151}">
-  <dimension ref="A1:AT3"/>
+  <dimension ref="A1:AT5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -610,7 +612,7 @@
     <col min="35" max="35" width="22.1640625" style="1" customWidth="1"/>
     <col min="36" max="36" width="24.6640625" style="1" customWidth="1"/>
     <col min="37" max="37" width="26.6640625" style="1" customWidth="1"/>
-    <col min="38" max="38" width="60.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="60.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="32" style="1" customWidth="1"/>
     <col min="40" max="40" width="27.1640625" style="1" customWidth="1"/>
     <col min="41" max="41" width="22.6640625" style="1" customWidth="1"/>
@@ -763,14 +765,14 @@
       </c>
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="C2" s="1">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1">
         <v>1.5</v>
@@ -779,7 +781,7 @@
         <v>80</v>
       </c>
       <c r="F2" s="1">
-        <v>165</v>
+        <v>77</v>
       </c>
       <c r="G2" s="1">
         <v>4</v>
@@ -788,10 +790,10 @@
         <v>10</v>
       </c>
       <c r="I2" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="J2" s="1">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="K2" s="1">
         <v>1.5</v>
@@ -821,7 +823,7 @@
         <v>0</v>
       </c>
       <c r="T2" s="1">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="U2" s="1">
         <v>10</v>
@@ -829,82 +831,87 @@
       <c r="V2" s="1">
         <v>15</v>
       </c>
-      <c r="W2" s="1">
+      <c r="W2" s="2">
+        <v>5</v>
+      </c>
+      <c r="X2" s="2">
+        <v>130</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>5000</v>
+      </c>
+      <c r="AA2" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="AB2" s="4">
+        <v>0.33</v>
+      </c>
+      <c r="AC2" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD2" s="2">
+        <v>8</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF2" s="1">
         <v>0</v>
       </c>
-      <c r="X2" s="1">
-        <v>15</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z2" s="1">
-        <v>9166.6666666666806</v>
-      </c>
-      <c r="AA2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="5">
-        <v>1</v>
-      </c>
-      <c r="AC2" s="1">
-        <v>20</v>
-      </c>
-      <c r="AD2" s="1">
-        <v>8</v>
-      </c>
-      <c r="AE2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AF2" s="1">
-        <v>82500</v>
-      </c>
-      <c r="AG2" s="1">
+      <c r="AG2" s="2">
         <v>12.2</v>
       </c>
-      <c r="AH2" s="1">
-        <v>4</v>
-      </c>
-      <c r="AI2" s="1">
+      <c r="AH2" s="2">
+        <v>10</v>
+      </c>
+      <c r="AI2" s="2">
         <v>2</v>
       </c>
-      <c r="AJ2" s="1">
+      <c r="AJ2" s="2">
         <v>1.4</v>
       </c>
       <c r="AK2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AL2" s="4">
-        <f>231750+1287500</f>
-        <v>1519250</v>
-      </c>
-      <c r="AM2" s="1">
+      <c r="AL2" s="5">
+        <v>0</v>
+      </c>
+      <c r="AM2" s="2">
         <v>0.03</v>
       </c>
-      <c r="AN2" s="1">
+      <c r="AN2" s="2">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="AO2" s="1">
+      <c r="AO2" s="2">
         <v>0</v>
       </c>
-      <c r="AP2" s="1">
+      <c r="AP2" s="2">
         <v>0.05</v>
       </c>
-      <c r="AQ2" s="1">
+      <c r="AQ2" s="2">
         <v>0.05</v>
       </c>
-      <c r="AR2" s="1">
+      <c r="AR2" s="2">
         <v>0</v>
       </c>
-      <c r="AS2" s="1">
+      <c r="AS2" s="2">
         <v>1</v>
       </c>
-      <c r="AT2" s="1">
+      <c r="AT2" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="Z3" s="2"/>
+      <c r="A3"/>
+    </row>
+    <row r="4" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="Z4" s="2"/>
+    </row>
+    <row r="5" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="Z5" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>